<commit_message>
update module test spec
</commit_message>
<xml_diff>
--- a/adhafera/test/module_test.xlsx
+++ b/adhafera/test/module_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -278,6 +278,105 @@
   </si>
   <si>
     <t>inputs: [null, null, null, null, null]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.getSettlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-01'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿が登録されている
+{
+  account_type: 'income',
+  date: '2015-01-01',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '2015-01-02',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 100
+}</t>
+    <rPh sb="0" eb="2">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="204" eb="205">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.getSettlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-01-01'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-02'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: ''</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿が登録されている
+{
+  account_type: 'income',
+  date: '2015-01-01',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '2015-01-02',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 100
+}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -334,7 +433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -474,19 +573,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -570,17 +656,89 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -772,20 +930,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -798,38 +955,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -925,6 +1127,7 @@
     <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1021,6 +1224,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="192" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1349,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1377,7 +1581,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1385,78 +1589,119 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="96">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="136" thickBot="1">
-      <c r="B6" s="14">
+    <row r="6" spans="2:7" ht="135">
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="24" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="102" customHeight="1">
+      <c r="B7" s="19">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="26">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="102" customHeight="1" thickBot="1">
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="25" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F7:F8"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1470,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G10"/>
+  <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1498,7 +1743,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1506,150 +1751,227 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="96">
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="16" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="96">
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="96">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="122">
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="123" thickBot="1">
-      <c r="B10" s="14">
+    <row r="10" spans="2:7" ht="122">
+      <c r="B10" s="19">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="24" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="51" customHeight="1">
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="51" customHeight="1">
+      <c r="B12" s="7">
+        <v>10</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="51" customHeight="1">
+      <c r="B13" s="19">
+        <v>11</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="51" customHeight="1" thickBot="1">
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F11:F14"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
settle on register (#84)
* upadte use case

* update requirement spec

* update ui

* output images for ui

* remove comment

* update functional spec

* update design umls

* update design spec

* update adhafera to 2.0.0

* update module test spec

* update system test spec
</commit_message>
<xml_diff>
--- a/adhafera/test/module_test.xlsx
+++ b/adhafera/test/module_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -278,6 +278,105 @@
   </si>
   <si>
     <t>inputs: [null, null, null, null, null]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.getSettlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-01'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿が登録されている
+{
+  account_type: 'income',
+  date: '2015-01-01',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '2015-01-02',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 100
+}</t>
+    <rPh sb="0" eb="2">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="204" eb="205">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.getSettlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-01-01'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: '2015-02'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>month: ''</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下の家計簿が登録されている
+{
+  account_type: 'income',
+  date: '2015-01-01',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 1000
+},
+{
+  account_type: 'expense',
+  date: '2015-01-02',
+  content: 'モジュールテスト用データ',
+  category: 'adhafera',
+  price: 100
+}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -334,7 +433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -474,19 +573,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -570,17 +656,89 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -772,20 +930,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -798,38 +955,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -925,6 +1127,7 @@
     <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1021,6 +1224,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="192" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1349,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1377,7 +1581,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1385,78 +1589,119 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="96">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="16" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="136" thickBot="1">
-      <c r="B6" s="14">
+    <row r="6" spans="2:7" ht="135">
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="24" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="102" customHeight="1">
+      <c r="B7" s="19">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="26">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="102" customHeight="1" thickBot="1">
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="25" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F7:F8"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1470,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G10"/>
+  <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1498,7 +1743,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1506,150 +1751,227 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="96">
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="16" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="96">
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="96">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="122">
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="123" thickBot="1">
-      <c r="B10" s="14">
+    <row r="10" spans="2:7" ht="122">
+      <c r="B10" s="19">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="24" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="51" customHeight="1">
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="51" customHeight="1">
+      <c r="B12" s="7">
+        <v>10</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="51" customHeight="1">
+      <c r="B13" s="19">
+        <v>11</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="51" customHeight="1" thickBot="1">
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F11:F14"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
modify module test case
</commit_message>
<xml_diff>
--- a/adhafera/test/module_test.xlsx
+++ b/adhafera/test/module_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -88,48 +88,6 @@
   </si>
   <si>
     <t>HTTPClient.sendRequest</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>inputs:[
-  '2015-01-01',
-  'テスト用データ',
-  'テスト',
-  '100',
-  'expense'
-]</t>
-    <rPh sb="31" eb="32">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{
-  status: 201,
-  body: {
-    account_type: 'expense',
-    date: '2015-01-01',
-    content: 'テスト用データ',
-    category: 'テスト',
-    price: 100
-  }
-}</t>
-    <rPh sb="97" eb="98">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>inputs:[
-  '2015-01-01',
-  'テスト用データ',
-  'テスト',
-  '100',
-  'expense'
-]</t>
-    <rPh sb="31" eb="32">
-      <t>ヨウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -286,10 +244,6 @@
   </si>
   <si>
     <t>HTTPClient.getSettlement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>month: '2015-01'</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -354,10 +308,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>month: '2015-02'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>month: ''</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -377,6 +327,48 @@
   category: 'adhafera',
   price: 100
 }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  statusCode: 201,
+  body: {
+    account_type: 'expense',
+    date: '2015-01-01',
+    content: 'テスト用データ',
+    category: 'テスト',
+    price: 100
+  }
+}</t>
+    <rPh sb="101" eb="102">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  statusCode: 200,
+  body: {
+    2015-01: 1000
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -433,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -737,6 +729,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -933,7 +938,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -997,12 +1002,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1024,10 +1023,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,7 +1564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G8"/>
+  <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1599,7 +1610,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
@@ -1653,55 +1664,32 @@
         <v>15</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="102" customHeight="1">
-      <c r="B7" s="19">
+    <row r="7" spans="2:7" ht="102" customHeight="1" thickBot="1">
+      <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="26">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="102" customHeight="1" thickBot="1">
-      <c r="B8" s="13">
-        <v>6</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="C7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="25" t="s">
-        <v>48</v>
+      <c r="E7" s="16"/>
+      <c r="F7" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F7:F8"/>
-  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1758,14 +1746,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -1776,14 +1764,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -1794,14 +1782,14 @@
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -1812,14 +1800,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="96">
@@ -1833,11 +1821,11 @@
         <v>15</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="96">
@@ -1848,14 +1836,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="122">
@@ -1866,14 +1854,14 @@
         <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="122">
@@ -1884,88 +1872,88 @@
         <v>5</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="51" customHeight="1">
       <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="F11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="51" customHeight="1">
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>46</v>
+      <c r="C12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="F12" s="33"/>
       <c r="G12" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="51" customHeight="1">
       <c r="B13" s="19">
         <v>11</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="30" t="s">
+      <c r="C13" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="51" customHeight="1" thickBot="1">
       <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify spec for adhafera (#85)
* modify module test case

* modify umls

* modify design_spec
</commit_message>
<xml_diff>
--- a/adhafera/test/module_test.xlsx
+++ b/adhafera/test/module_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -88,48 +88,6 @@
   </si>
   <si>
     <t>HTTPClient.sendRequest</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>inputs:[
-  '2015-01-01',
-  'テスト用データ',
-  'テスト',
-  '100',
-  'expense'
-]</t>
-    <rPh sb="31" eb="32">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{
-  status: 201,
-  body: {
-    account_type: 'expense',
-    date: '2015-01-01',
-    content: 'テスト用データ',
-    category: 'テスト',
-    price: 100
-  }
-}</t>
-    <rPh sb="97" eb="98">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>inputs:[
-  '2015-01-01',
-  'テスト用データ',
-  'テスト',
-  '100',
-  'expense'
-]</t>
-    <rPh sb="31" eb="32">
-      <t>ヨウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -286,10 +244,6 @@
   </si>
   <si>
     <t>HTTPClient.getSettlement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>month: '2015-01'</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -354,10 +308,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>month: '2015-02'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>month: ''</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -377,6 +327,48 @@
   category: 'adhafera',
   price: 100
 }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  statusCode: 201,
+  body: {
+    account_type: 'expense',
+    date: '2015-01-01',
+    content: 'テスト用データ',
+    category: 'テスト',
+    price: 100
+  }
+}</t>
+    <rPh sb="101" eb="102">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  statusCode: 200,
+  body: {
+    2015-01: 1000
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -433,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -737,6 +729,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -933,7 +938,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -997,12 +1002,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1024,10 +1023,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,7 +1564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G8"/>
+  <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1599,7 +1610,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
@@ -1653,55 +1664,32 @@
         <v>15</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="102" customHeight="1">
-      <c r="B7" s="19">
+    <row r="7" spans="2:7" ht="102" customHeight="1" thickBot="1">
+      <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="26">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="102" customHeight="1" thickBot="1">
-      <c r="B8" s="13">
-        <v>6</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="C7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="25" t="s">
-        <v>48</v>
+      <c r="E7" s="16"/>
+      <c r="F7" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F7:F8"/>
-  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1758,14 +1746,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -1776,14 +1764,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -1794,14 +1782,14 @@
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -1812,14 +1800,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="96">
@@ -1833,11 +1821,11 @@
         <v>15</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="96">
@@ -1848,14 +1836,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="122">
@@ -1866,14 +1854,14 @@
         <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="122">
@@ -1884,88 +1872,88 @@
         <v>5</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="51" customHeight="1">
       <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="F11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="51" customHeight="1">
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>46</v>
+      <c r="C12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="F12" s="33"/>
       <c r="G12" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="51" customHeight="1">
       <c r="B13" s="19">
         <v>11</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="30" t="s">
+      <c r="C13" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="51" customHeight="1" thickBot="1">
       <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>